<commit_message>
added fucntioanlity to get tests
</commit_message>
<xml_diff>
--- a/src/excely/DVP_template_empty.xlsx
+++ b/src/excely/DVP_template_empty.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MatFyz\V_SEMESTER\BOGE\form-versions\src\excely\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145E94CC-F3FF-400C-B952-33EC8B8BF316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4497242D-2A7A-4F57-8FB1-B8E6BC7C53FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22810" yWindow="-15670" windowWidth="32580" windowHeight="17990" tabRatio="603" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-18570" windowWidth="38620" windowHeight="21100" tabRatio="603" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DVP Internal" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="123">
   <si>
     <r>
       <t>F</t>
@@ -657,21 +657,6 @@
     <t>ok</t>
   </si>
   <si>
-    <t>273.000.013.459A</t>
-  </si>
-  <si>
-    <t>273.000.013.459B</t>
-  </si>
-  <si>
-    <t>273.000.013.459V</t>
-  </si>
-  <si>
-    <t>273.000.013.459C</t>
-  </si>
-  <si>
-    <t>273.000.013.459D</t>
-  </si>
-  <si>
     <t>6M0.412.377.F EM10</t>
   </si>
   <si>
@@ -681,7 +666,7 @@
     <t>5/14/2019</t>
   </si>
   <si>
-    <t>5/14/2020</t>
+    <t>273.401.012.379C</t>
   </si>
 </sst>
 </file>
@@ -2551,9 +2536,6 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2561,6 +2543,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="10" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3835,7 +3820,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Verhältnisrech."/>
@@ -3848,7 +3833,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Verhältnisrech."/>
@@ -4183,11 +4168,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CU148"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="4" ySplit="7" topLeftCell="CH8" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="4" ySplit="7" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="CF2" sqref="CF2:CI2"/>
+      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" outlineLevelCol="2"/>
@@ -4304,16 +4289,16 @@
       <c r="H2" s="279"/>
       <c r="I2" s="279"/>
       <c r="J2" s="280"/>
-      <c r="K2" s="300" t="s">
+      <c r="K2" s="299" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="301"/>
-      <c r="M2" s="301"/>
-      <c r="N2" s="302"/>
+      <c r="L2" s="300"/>
+      <c r="M2" s="300"/>
+      <c r="N2" s="301"/>
       <c r="O2" s="284" t="s">
         <v>44</v>
       </c>
-      <c r="P2" s="299" t="s">
+      <c r="P2" s="302" t="s">
         <v>92</v>
       </c>
       <c r="Q2" s="291"/>
@@ -4330,7 +4315,7 @@
       <c r="Z2" s="284" t="s">
         <v>100</v>
       </c>
-      <c r="AA2" s="299" t="s">
+      <c r="AA2" s="302" t="s">
         <v>94</v>
       </c>
       <c r="AB2" s="291"/>
@@ -5364,7 +5349,7 @@
         <v>116</v>
       </c>
       <c r="C9" s="259" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="D9" s="260" t="s">
         <v>117</v>
@@ -5487,14 +5472,14 @@
       <c r="CN9" s="80"/>
     </row>
     <row r="10" spans="1:99" ht="13.8" thickBot="1">
-      <c r="A10" s="259" t="s">
-        <v>127</v>
+      <c r="A10" s="259">
+        <v>44083</v>
       </c>
       <c r="B10" s="259" t="s">
         <v>116</v>
       </c>
       <c r="C10" s="259" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="D10" s="260" t="s">
         <v>117</v>
@@ -5567,7 +5552,7 @@
       <c r="AZ10" s="33"/>
       <c r="BA10" s="70"/>
       <c r="BB10" s="234" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="BC10" s="234"/>
       <c r="BD10" s="234"/>
@@ -5622,13 +5607,13 @@
     </row>
     <row r="11" spans="1:99" ht="13.8" thickBot="1">
       <c r="A11" s="259">
-        <v>44113</v>
+        <v>44083</v>
       </c>
       <c r="B11" s="259" t="s">
         <v>116</v>
       </c>
       <c r="C11" s="259" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="D11" s="260" t="s">
         <v>117</v>
@@ -5738,13 +5723,13 @@
     </row>
     <row r="12" spans="1:99" ht="13.8" thickBot="1">
       <c r="A12" s="259">
-        <v>44020</v>
+        <v>44083</v>
       </c>
       <c r="B12" s="259" t="s">
         <v>116</v>
       </c>
       <c r="C12" s="259" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="D12" s="260" t="s">
         <v>117</v>
@@ -5762,7 +5747,7 @@
       </c>
       <c r="N12" s="34"/>
       <c r="O12" s="234" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="P12" s="180"/>
       <c r="Q12" s="181"/>
@@ -5812,7 +5797,7 @@
       <c r="BA12" s="70"/>
       <c r="BB12" s="234"/>
       <c r="BC12" s="234" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="BD12" s="234"/>
       <c r="BE12" s="234"/>
@@ -5828,7 +5813,7 @@
       <c r="BM12" s="46"/>
       <c r="BN12" s="22"/>
       <c r="BO12" s="234" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="BP12" s="29"/>
       <c r="BQ12" s="22"/>
@@ -5843,7 +5828,7 @@
       <c r="BV12" s="20"/>
       <c r="BW12" s="22"/>
       <c r="BX12" s="234" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="BY12" s="29">
         <v>234</v>
@@ -5874,10 +5859,10 @@
         <v>116</v>
       </c>
       <c r="C13" s="259" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D13" s="260" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E13" s="160"/>
       <c r="F13" s="160"/>
@@ -5988,10 +5973,10 @@
         <v>116</v>
       </c>
       <c r="C14" s="259" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D14" s="260" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E14" s="160"/>
       <c r="F14" s="160"/>
@@ -6006,7 +5991,7 @@
       <c r="M14" s="66"/>
       <c r="N14" s="34"/>
       <c r="O14" s="234" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="P14" s="180"/>
       <c r="Q14" s="181"/>
@@ -6070,7 +6055,7 @@
       </c>
       <c r="BJ14" s="22"/>
       <c r="BK14" s="234" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="BL14" s="46"/>
       <c r="BM14" s="46"/>
@@ -6114,16 +6099,16 @@
     </row>
     <row r="15" spans="1:99" ht="13.8" thickBot="1">
       <c r="A15" s="259" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B15" s="259" t="s">
         <v>116</v>
       </c>
       <c r="C15" s="259" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D15" s="260" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E15" s="160"/>
       <c r="F15" s="160"/>
@@ -6163,7 +6148,7 @@
       <c r="AL15" s="66"/>
       <c r="AM15" s="66"/>
       <c r="AN15" s="79" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="AO15" s="83"/>
       <c r="AP15" s="66"/>
@@ -6237,7 +6222,7 @@
         <v>122</v>
       </c>
       <c r="D16" s="260" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E16" s="160"/>
       <c r="F16" s="160"/>
@@ -6354,7 +6339,7 @@
         <v>116</v>
       </c>
       <c r="C17" s="259" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D17" s="260" t="s">
         <v>117</v>
@@ -18783,19 +18768,17 @@
   </sheetData>
   <autoFilter ref="A1:A8" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="43">
+    <mergeCell ref="AA2:AD2"/>
+    <mergeCell ref="BF2:BG2"/>
+    <mergeCell ref="BI2:BJ2"/>
+    <mergeCell ref="BE2:BE4"/>
+    <mergeCell ref="AU2:AW2"/>
+    <mergeCell ref="AR2:AT2"/>
+    <mergeCell ref="AX2:BA2"/>
     <mergeCell ref="CF2:CI2"/>
     <mergeCell ref="BH2:BH4"/>
     <mergeCell ref="CA2:CA4"/>
     <mergeCell ref="BB2:BB4"/>
-    <mergeCell ref="AA2:AD2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="P2:S2"/>
-    <mergeCell ref="BE2:BE4"/>
-    <mergeCell ref="AU2:AW2"/>
-    <mergeCell ref="AR2:AT2"/>
-    <mergeCell ref="AX2:BA2"/>
-    <mergeCell ref="BF2:BG2"/>
-    <mergeCell ref="BI2:BJ2"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="E3:E7"/>
     <mergeCell ref="AO3:AP3"/>
@@ -18810,6 +18793,8 @@
     <mergeCell ref="AJ3:AK3"/>
     <mergeCell ref="AH3:AI3"/>
     <mergeCell ref="F3:G3"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="P2:S2"/>
     <mergeCell ref="CN3:CN4"/>
     <mergeCell ref="AR3:AS3"/>
     <mergeCell ref="AU3:AV3"/>

</xml_diff>